<commit_message>
Added user stories documentation
Added user stories documentation
</commit_message>
<xml_diff>
--- a/Docs/Program Management/Agile Scrum Project Management.xlsx
+++ b/Docs/Program Management/Agile Scrum Project Management.xlsx
@@ -179,12 +179,6 @@
     <t>A school cafeteria manager would like to access the latest food recall list, print the list on a weekly basis and share it with cafeteria staff on a weekly basis</t>
   </si>
   <si>
-    <t>Using human-centered design approach, create the PERSONA, SCENARIO and USE-CASES</t>
-  </si>
-  <si>
-    <t>Using the persona, scenario, use-cases and input from users create the initial wireframes</t>
-  </si>
-  <si>
     <t>Iteratively evolve the wireframes getting feedback from users</t>
   </si>
   <si>
@@ -194,16 +188,10 @@
     <t>Incorporate suggestion/feedback from the paper-based usability testing into wireframes</t>
   </si>
   <si>
-    <t>Develop HTML templates from the evolved wireframes</t>
-  </si>
-  <si>
     <t>Conduct Usability testing on html templates</t>
   </si>
   <si>
     <t>Incorporate changes to templates with feedback from Usability testing</t>
-  </si>
-  <si>
-    <t>Develop prototype application using the latest html templates, using TDD and continuous integration/deployment environment setup</t>
   </si>
   <si>
     <t>SPRINT</t>
@@ -360,6 +348,18 @@
   </si>
   <si>
     <t>Review and test  prototype after every nightly build, going through feedback/suggestion. With agreement of product manager add it to  Task list for engineers to take care</t>
+  </si>
+  <si>
+    <t>Develop prototype application (implementing user stories 1,2,3 using the latest html templates, using TDD and continuous integration/deployment environment setup</t>
+  </si>
+  <si>
+    <t>Develop HTML templates from the evolved wireframes for user stories 1, 2,3</t>
+  </si>
+  <si>
+    <t>Using the persona, scenario, use-cases and input from users to create the initial wireframes for user stories 1,2,3</t>
+  </si>
+  <si>
+    <t>Using human-centered design approach, create the PERSONA, SCENARIO and USE-CASES for user stories 1, 2, 3</t>
   </si>
 </sst>
 </file>
@@ -1410,8 +1410,8 @@
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>371475</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>212725</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1465,8 +1465,8 @@
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>381000</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>31750</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1521,7 +1521,7 @@
       <xdr:col>6</xdr:col>
       <xdr:colOff>409575</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:rowOff>6350</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3243,7 +3243,7 @@
   <sheetData>
     <row r="1" spans="1:1" ht="21" x14ac:dyDescent="0.5">
       <c r="A1" s="14" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="217.5" x14ac:dyDescent="0.35">
@@ -3294,7 +3294,7 @@
     </row>
     <row r="2" spans="1:13" ht="18.600000000000001" x14ac:dyDescent="0.45">
       <c r="A2" s="18" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B2" s="53"/>
       <c r="C2" s="53"/>
@@ -3631,7 +3631,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="21" x14ac:dyDescent="0.5">
       <c r="A1" s="55" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B1" s="55"/>
     </row>
@@ -3716,7 +3716,7 @@
   <sheetData>
     <row r="1" spans="1:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B1" s="54" t="s">
         <v>9</v>
@@ -3883,7 +3883,7 @@
     </row>
     <row r="9" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B9" s="26"/>
       <c r="C9" s="22"/>
@@ -3902,7 +3902,7 @@
     </row>
     <row r="10" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B10" s="34"/>
       <c r="C10" s="35"/>
@@ -3946,7 +3946,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="21" x14ac:dyDescent="0.5">
       <c r="A1" s="55" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B1" s="55"/>
     </row>
@@ -3986,8 +3986,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N20"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView topLeftCell="A13" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4000,10 +4000,10 @@
   <sheetData>
     <row r="1" spans="1:14" ht="18.600000000000001" x14ac:dyDescent="0.35">
       <c r="A1" s="13" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C1" s="54" t="s">
         <v>9</v>
@@ -4022,7 +4022,7 @@
     </row>
     <row r="2" spans="1:14" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A2" s="57" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B2" s="57"/>
       <c r="C2" s="7">
@@ -4064,10 +4064,10 @@
     </row>
     <row r="3" spans="1:14" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A3" s="44" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B3" s="45" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C3" s="41"/>
       <c r="D3" s="39"/>
@@ -4084,10 +4084,10 @@
     </row>
     <row r="4" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="44" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B4" s="45" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C4" s="26"/>
       <c r="D4" s="22"/>
@@ -4104,10 +4104,10 @@
     </row>
     <row r="5" spans="1:14" ht="29.1" x14ac:dyDescent="0.35">
       <c r="A5" s="44" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B5" s="45" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C5" s="26"/>
       <c r="D5" s="22"/>
@@ -4124,7 +4124,7 @@
     </row>
     <row r="6" spans="1:14" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A6" s="58" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B6" s="58"/>
       <c r="C6" s="26"/>
@@ -4142,10 +4142,10 @@
     </row>
     <row r="7" spans="1:14" ht="58.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="44" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B7" s="45" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C7" s="26"/>
       <c r="D7" s="22"/>
@@ -4162,10 +4162,10 @@
     </row>
     <row r="8" spans="1:14" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="44" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B8" s="45" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C8" s="26"/>
       <c r="D8" s="22"/>
@@ -4182,10 +4182,10 @@
     </row>
     <row r="9" spans="1:14" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="44" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B9" s="45" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C9" s="26"/>
       <c r="D9" s="22"/>
@@ -4202,10 +4202,10 @@
     </row>
     <row r="10" spans="1:14" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="44" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B10" s="45" t="s">
-        <v>43</v>
+        <v>101</v>
       </c>
       <c r="C10" s="26"/>
       <c r="D10" s="22"/>
@@ -4222,10 +4222,10 @@
     </row>
     <row r="11" spans="1:14" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="44" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B11" s="45" t="s">
-        <v>44</v>
+        <v>100</v>
       </c>
       <c r="C11" s="26"/>
       <c r="D11" s="22"/>
@@ -4242,10 +4242,10 @@
     </row>
     <row r="12" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="44" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B12" s="45" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C12" s="26"/>
       <c r="D12" s="22"/>
@@ -4262,10 +4262,10 @@
     </row>
     <row r="13" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="44" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B13" s="45" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C13" s="26"/>
       <c r="D13" s="22"/>
@@ -4282,10 +4282,10 @@
     </row>
     <row r="14" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="44" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B14" s="45" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C14" s="26"/>
       <c r="D14" s="22"/>
@@ -4300,12 +4300,12 @@
       <c r="M14" s="22"/>
       <c r="N14" s="23"/>
     </row>
-    <row r="15" spans="1:14" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="44" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B15" s="45" t="s">
-        <v>48</v>
+        <v>99</v>
       </c>
       <c r="C15" s="26"/>
       <c r="D15" s="22"/>
@@ -4320,12 +4320,12 @@
       <c r="M15" s="22"/>
       <c r="N15" s="23"/>
     </row>
-    <row r="16" spans="1:14" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="44" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B16" s="45" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C16" s="26"/>
       <c r="D16" s="22"/>
@@ -4340,12 +4340,12 @@
       <c r="M16" s="22"/>
       <c r="N16" s="23"/>
     </row>
-    <row r="17" spans="1:14" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="44" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B17" s="45" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C17" s="26"/>
       <c r="D17" s="22"/>
@@ -4360,12 +4360,12 @@
       <c r="M17" s="22"/>
       <c r="N17" s="23"/>
     </row>
-    <row r="18" spans="1:14" ht="35.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:14" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="44" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B18" s="45" t="s">
-        <v>51</v>
+        <v>98</v>
       </c>
       <c r="C18" s="26"/>
       <c r="D18" s="22"/>
@@ -4382,10 +4382,10 @@
     </row>
     <row r="19" spans="1:14" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="44" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B19" s="45" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C19" s="26"/>
       <c r="D19" s="22"/>
@@ -4400,12 +4400,12 @@
       <c r="M19" s="22"/>
       <c r="N19" s="23"/>
     </row>
-    <row r="20" spans="1:14" ht="35.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:14" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="44" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B20" s="45" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C20" s="34"/>
       <c r="D20" s="35"/>
@@ -4435,7 +4435,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
@@ -4451,22 +4451,22 @@
   <sheetData>
     <row r="1" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="16" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C1" s="17" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D1" s="17" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="E1" s="17" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="F1" s="52" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="14.45" x14ac:dyDescent="0.35">
@@ -4474,16 +4474,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="45" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C2" s="44" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="D2" s="44" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="E2" s="50" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="F2" s="45"/>
     </row>
@@ -4492,16 +4492,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="45" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C3" s="44" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="D3" s="44" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="E3" s="50" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="F3" s="45"/>
     </row>
@@ -4510,16 +4510,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="45" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C4" s="44" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="D4" s="44" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="E4" s="50" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="F4" s="45"/>
     </row>
@@ -4528,16 +4528,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="45" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C5" s="44" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="D5" s="44" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="E5" s="50" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="F5" s="45"/>
     </row>
@@ -4546,16 +4546,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="45" t="s">
+        <v>63</v>
+      </c>
+      <c r="C6" s="44" t="s">
+        <v>84</v>
+      </c>
+      <c r="D6" s="44" t="s">
         <v>67</v>
       </c>
-      <c r="C6" s="44" t="s">
-        <v>88</v>
-      </c>
-      <c r="D6" s="44" t="s">
-        <v>71</v>
-      </c>
       <c r="E6" s="50" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="F6" s="45"/>
     </row>
@@ -4564,16 +4564,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="45" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C7" s="44" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="D7" s="44" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="E7" s="50" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="F7" s="45"/>
     </row>
@@ -4582,13 +4582,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="45" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C8" s="44" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="D8" s="44" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="E8" s="50"/>
       <c r="F8" s="45"/>
@@ -4598,13 +4598,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="45" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C9" s="44" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="D9" s="44" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="E9" s="50"/>
       <c r="F9" s="45"/>
@@ -4614,16 +4614,16 @@
         <v>9</v>
       </c>
       <c r="B10" s="45" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C10" s="44" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="D10" s="44" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="E10" s="50" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="F10" s="45"/>
     </row>
@@ -4632,16 +4632,16 @@
         <v>10</v>
       </c>
       <c r="B11" s="45" t="s">
+        <v>79</v>
+      </c>
+      <c r="C11" s="44" t="s">
         <v>83</v>
       </c>
-      <c r="C11" s="44" t="s">
-        <v>87</v>
-      </c>
       <c r="D11" s="44" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="E11" s="50" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="F11" s="45"/>
     </row>
@@ -4650,16 +4650,16 @@
         <v>11</v>
       </c>
       <c r="B12" s="45" t="s">
+        <v>80</v>
+      </c>
+      <c r="C12" s="44" t="s">
         <v>84</v>
       </c>
-      <c r="C12" s="44" t="s">
-        <v>88</v>
-      </c>
       <c r="D12" s="44" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="E12" s="50" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="F12" s="45"/>
     </row>
@@ -4668,16 +4668,16 @@
         <v>12</v>
       </c>
       <c r="B13" s="45" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C13" s="44" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="D13" s="44" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="E13" s="50" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="F13" s="45"/>
     </row>
@@ -4686,16 +4686,16 @@
         <v>13</v>
       </c>
       <c r="B14" s="45" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C14" s="44" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="D14" s="44" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="E14" s="50" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="F14" s="45"/>
     </row>
@@ -4704,16 +4704,16 @@
         <v>14</v>
       </c>
       <c r="B15" s="48" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C15" s="47" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="D15" s="47" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="E15" s="41" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="F15" s="45"/>
     </row>
@@ -4722,17 +4722,17 @@
         <v>15</v>
       </c>
       <c r="B16" s="45" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C16" s="49" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="D16" s="49" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="E16" s="50"/>
       <c r="F16" s="45" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="14.45" x14ac:dyDescent="0.35">
@@ -4740,22 +4740,22 @@
         <v>16</v>
       </c>
       <c r="B17" s="45" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C17" s="49" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="D17" s="49" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="E17" s="51" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="F17" s="45"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E22" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>